<commit_message>
Added hint and fixes codword validation
</commit_message>
<xml_diff>
--- a/Documentation/Sample Data/Codewords.xlsx
+++ b/Documentation/Sample Data/Codewords.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834E66DF-9E50-4BF5-9D1D-801B293638F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
   <si>
     <t>Codeword</t>
   </si>
@@ -304,7 +303,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -664,11 +663,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,6 +1247,11 @@
         <v>28</v>
       </c>
     </row>
+    <row r="116" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>